<commit_message>
finished upload post process and converted csv to JSOn
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\us53807\Documents\Roopa\gt-enrich\gt-enrich-server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\us53807\Documents\Roopa\gt-enrich-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9528"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -199,10 +199,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="168" formatCode="#0"/>
-    <numFmt numFmtId="169" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="170" formatCode="#0.00"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#0.00"/>
+    <numFmt numFmtId="164" formatCode="#0"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="#0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -261,10 +261,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -273,10 +273,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -595,9 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>